<commit_message>
Completed Flavor text and progression
Finished doing all the writing for the first area and dungeon. Now just
need to get with greg to implement the characture stats and the talent
trees. If we can get that done soon I will start creating items.
</commit_message>
<xml_diff>
--- a/public/assets/Game play info (thomas)/Starting hero.xlsx
+++ b/public/assets/Game play info (thomas)/Starting hero.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="13395" windowHeight="4425"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="13395" windowHeight="4425" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1336,7 +1336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -1658,8 +1658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>